<commit_message>
ya entregue el proyecto final
</commit_message>
<xml_diff>
--- a/I. 02 Análisis Estadístico I/Practicas/ProyectoFinal/indices.xlsx
+++ b/I. 02 Análisis Estadístico I/Practicas/ProyectoFinal/indices.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rserdan\Desktop\MCD\I. 02 Análisis Estadístico I\Practicas\ProyectoFinal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilde\Desktop\MCD\I. 02 Análisis Estadístico I\Practicas\ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,21 +24,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="7">
   <si>
-    <t>IndiceTotal</t>
+    <t>Fecha</t>
   </si>
   <si>
-    <t>IndiceMinerales</t>
+    <t>Valor</t>
   </si>
   <si>
-    <t>IndiceAgricolas</t>
+    <t>MINERALES</t>
   </si>
   <si>
-    <t>IndiceCombustibles</t>
+    <t>AGRICOLAS</t>
   </si>
   <si>
-    <t>Fecha</t>
+    <t>HIDROCARBUROS</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Tipo</t>
   </si>
 </sst>
 </file>
@@ -358,204 +364,466 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44197</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
         <v>135.0203697167079</v>
       </c>
-      <c r="C2" s="2">
-        <v>171.22357909907194</v>
-      </c>
-      <c r="D2" s="2">
-        <v>97.729356137513435</v>
-      </c>
-      <c r="E2" s="2">
-        <v>116.17306977538531</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44228</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
         <v>139.75567850975233</v>
       </c>
-      <c r="C3" s="2">
-        <v>172.05862773912378</v>
-      </c>
-      <c r="D3" s="2">
-        <v>100.03007253611051</v>
-      </c>
-      <c r="E3" s="2">
-        <v>119.06019982187081</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44256</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
         <v>137.12624038207252</v>
       </c>
-      <c r="C4" s="2">
-        <v>174.9563394526653</v>
-      </c>
-      <c r="D4" s="2">
-        <v>101.69797729062834</v>
-      </c>
-      <c r="E4" s="2">
-        <v>119.55916809029409</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44287</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
         <v>140.14006588383117</v>
       </c>
-      <c r="C5" s="2">
-        <v>173.39802046630729</v>
-      </c>
-      <c r="D5" s="2">
-        <v>115.86261916312341</v>
-      </c>
-      <c r="E5" s="2">
-        <v>128.8254210708202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44317</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
         <v>150.45739166790241</v>
       </c>
-      <c r="C6" s="2">
-        <v>180.93785987459236</v>
-      </c>
-      <c r="D6" s="2">
-        <v>116.90400670135635</v>
-      </c>
-      <c r="E6" s="2">
-        <v>133.29261762251156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44348</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2">
         <v>150.49153352611543</v>
       </c>
-      <c r="C7" s="2">
-        <v>174.62385835077038</v>
-      </c>
-      <c r="D7" s="2">
-        <v>119.85750365944696</v>
-      </c>
-      <c r="E7" s="2">
-        <v>134.45570645343199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44378</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
         <v>151.1337836413868</v>
       </c>
-      <c r="C8" s="2">
-        <v>175.97573333072842</v>
-      </c>
-      <c r="D8" s="2">
-        <v>134.77188559985413</v>
-      </c>
-      <c r="E8" s="2">
-        <v>143.74762372568429</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44409</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2">
         <v>150.38298275971462</v>
       </c>
-      <c r="C9" s="2">
-        <v>173.06692277117148</v>
-      </c>
-      <c r="D9" s="2">
-        <v>133.52889170320472</v>
-      </c>
-      <c r="E9" s="2">
-        <v>142.48812896127856</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44440</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2">
         <v>149.52929978349437</v>
       </c>
-      <c r="C10" s="2">
-        <v>169.0328722463691</v>
-      </c>
-      <c r="D10" s="2">
-        <v>134.83206177496518</v>
-      </c>
-      <c r="E10" s="2">
-        <v>142.61740543239736</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44470</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2">
         <v>154.37948038514259</v>
       </c>
-      <c r="C11" s="2">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>171.22357909907194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2">
+        <v>172.05862773912378</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>174.9563394526653</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2">
+        <v>173.39802046630729</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>180.93785987459236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2">
+        <v>174.62385835077038</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2">
+        <v>175.97573333072842</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2">
+        <v>173.06692277117148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2">
+        <v>169.0328722463691</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2">
         <v>175.50107952793823</v>
       </c>
-      <c r="D11" s="2">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="2">
+        <v>97.729356137513435</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="2">
+        <v>100.03007253611051</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="2">
+        <v>101.69797729062834</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2">
+        <v>115.86261916312341</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="2">
+        <v>116.90400670135635</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="2">
+        <v>119.85750365944696</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2">
+        <v>134.77188559985413</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="2">
+        <v>133.52889170320472</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="2">
+        <v>134.83206177496518</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="2">
         <v>119.75293946699587</v>
       </c>
-      <c r="E11" s="2">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="2">
+        <v>116.17306977538531</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="2">
+        <v>119.06019982187081</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="2">
+        <v>119.55916809029409</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="2">
+        <v>128.8254210708202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="2">
+        <v>133.29261762251156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="2">
+        <v>134.45570645343199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="2">
+        <v>143.74762372568429</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="2">
+        <v>142.48812896127856</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="2">
+        <v>142.61740543239736</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="2">
         <v>135.64665374144482</v>
       </c>
     </row>

</xml_diff>